<commit_message>
2.0.1 - Formula refinements
Updated Dashboard 'Application Status Breakdown' formulas.
</commit_message>
<xml_diff>
--- a/JobSearchAnalytics_Demo.xlsx
+++ b/JobSearchAnalytics_Demo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b7e2be8640e0f68/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7b7e2be8640e0f68/Desktop/Job Search Analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_433FEA0F33A9C9BCC33567341E2A68C5F0885CC7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD90F09A-B0C6-47D6-A28F-721B4CCED710}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="11_433FEA0F33A9C9BCC33567341E2A68C5F0885CC7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BFA5B0F6-4E66-4741-B5B8-E3E7C086E05B}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="500" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="375" yWindow="585" windowWidth="21600" windowHeight="18435" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="347">
   <si>
     <t>Job Search Analytics System</t>
   </si>
@@ -1079,6 +1079,21 @@
   </si>
   <si>
     <t xml:space="preserve">    MsgBox "Skills extracted successfully.", vbInformation, "Extraction Complete"</t>
+  </si>
+  <si>
+    <t>Versioning Legend</t>
+  </si>
+  <si>
+    <t>Architecture (X.0.0)  – Structural redesign or core workflow changes</t>
+  </si>
+  <si>
+    <t>Feature (0.X.0)  – New features, dashboards, or metrics added</t>
+  </si>
+  <si>
+    <t>Refinement (0.0.X)  – Fixes, formula updates, layout or wording improvements</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
   </si>
 </sst>
 </file>
@@ -1090,7 +1105,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1103,166 +1118,181 @@
       <sz val="30"/>
       <color rgb="FFC9D1D3"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF4F8A8B"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF4F8A8B"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FFC9D1D3"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF4F8A8B"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="13"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF1E1E1E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="24"/>
       <color rgb="FF7FB77E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFC9D1D3"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFC9D1D3"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF7FB77E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFC9D1D3"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFE8C07D"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF4F8A8B"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF1E1E1E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color rgb="FF4F8A8B"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF1E1E1E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF1E1E1E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF3A4A5A"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="22"/>
       <color rgb="FF7FB77E"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color rgb="FF1E1E1E"/>
       <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1417,7 +1447,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1549,34 +1579,10 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1585,6 +1591,30 @@
     <xf numFmtId="165" fontId="11" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1592,6 +1622,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1604,12 +1637,11 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,7 +1781,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -1938,7 +1970,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2023,7 +2055,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2150,7 +2182,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2444,7 +2476,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2529,7 +2561,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2656,7 +2688,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -2845,7 +2877,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2930,7 +2962,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3057,7 +3089,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3351,7 +3383,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3436,7 +3468,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3563,7 +3595,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3658,28 +3690,28 @@
                 <c:formatCode>mm/dd/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>46021</c:v>
+                  <c:v>46026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46028</c:v>
+                  <c:v>46033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46035</c:v>
+                  <c:v>46040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46042</c:v>
+                  <c:v>46047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46049</c:v>
+                  <c:v>46054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46056</c:v>
+                  <c:v>46061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46063</c:v>
+                  <c:v>46068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46070</c:v>
+                  <c:v>46075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3706,13 +3738,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3794,28 +3826,28 @@
                 <c:formatCode>mm/dd/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>46021</c:v>
+                  <c:v>46026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46028</c:v>
+                  <c:v>46033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46035</c:v>
+                  <c:v>46040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46042</c:v>
+                  <c:v>46047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46049</c:v>
+                  <c:v>46054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46056</c:v>
+                  <c:v>46061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46063</c:v>
+                  <c:v>46068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46070</c:v>
+                  <c:v>46075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3842,10 +3874,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -3930,28 +3962,28 @@
                 <c:formatCode>mm/dd/yyyy</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>46021</c:v>
+                  <c:v>46026</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46028</c:v>
+                  <c:v>46033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>46035</c:v>
+                  <c:v>46040</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46042</c:v>
+                  <c:v>46047</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>46049</c:v>
+                  <c:v>46054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46056</c:v>
+                  <c:v>46061</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>46063</c:v>
+                  <c:v>46068</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>46070</c:v>
+                  <c:v>46075</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4037,7 +4069,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4121,7 +4153,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4248,7 +4280,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1800" b="1" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1800" b="1" strike="noStrike" spc="-1">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -4492,7 +4524,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="1000" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="1000" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4704,15 +4736,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>146880</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>189000</xdr:rowOff>
+      <xdr:colOff>346905</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>55650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5137,13 +5169,16 @@
   </sheetPr>
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="11" max="11" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -5293,7 +5328,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -5328,7 +5363,9 @@
         <v>3</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
+      <c r="E14" s="73" t="s">
+        <v>342</v>
+      </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -5342,10 +5379,12 @@
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>5</v>
+        <v>346</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
+      <c r="E15" s="72" t="s">
+        <v>343</v>
+      </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -5362,7 +5401,9 @@
         <v>7</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
+      <c r="E16" s="72" t="s">
+        <v>344</v>
+      </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -5377,10 +5418,12 @@
       </c>
       <c r="C17" s="4" t="str">
         <f ca="1">TEXT(TODAY(),"MMMM DD, YYYY")</f>
-        <v>February 24, 2026</v>
+        <v>March 01, 2026</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
+      <c r="E17" s="72" t="s">
+        <v>345</v>
+      </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -5824,9 +5867,9 @@
   </sheetPr>
   <dimension ref="A1:M500"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:M1"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5836,7 +5879,7 @@
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
-    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="6" max="6" width="30.85546875" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
@@ -9092,7 +9135,9 @@
   </sheetPr>
   <dimension ref="A1:W79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9129,21 +9174,21 @@
     </row>
     <row r="2" spans="1:23" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14"/>
-      <c r="B2" s="60" t="s">
+      <c r="B2" s="51" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="60"/>
-      <c r="N2" s="60"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
       <c r="O2" s="14"/>
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
@@ -9181,24 +9226,24 @@
     </row>
     <row r="4" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
-      <c r="I4" s="53"/>
-      <c r="J4" s="53"/>
-      <c r="K4" s="53"/>
-      <c r="L4" s="53"/>
-      <c r="M4" s="53"/>
-      <c r="N4" s="53"/>
-      <c r="O4" s="53"/>
-      <c r="P4" s="53"/>
-      <c r="Q4" s="53"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="T4" s="14"/>
@@ -9233,34 +9278,34 @@
     </row>
     <row r="6" spans="1:23" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="B6" s="61">
+      <c r="B6" s="53">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;TODAY()-7)</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53">
+        <f ca="1">COUNTIFS(Log!H:H,"&lt;"&amp;TODAY(),Log!G:G,"Applied")</f>
         <v>2</v>
       </c>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61">
-        <f ca="1">COUNTIFS(Log!H:H,"&lt;"&amp;TODAY(),Log!G:G,"Applied")</f>
-        <v>1</v>
-      </c>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="62">
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="54">
         <f>IFERROR(COUNTIF(Log!G:G,"Interview Scheduled")/(COUNTA(Log!A:A)-1),0)</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="62"/>
-      <c r="M6" s="62"/>
-      <c r="N6" s="62">
+      <c r="K6" s="54"/>
+      <c r="L6" s="54"/>
+      <c r="M6" s="54"/>
+      <c r="N6" s="54">
         <f>IFERROR(COUNTIF(Log!G:G,"Offer")/(COUNTA(Log!A:A)-1),0)</f>
         <v>0</v>
       </c>
-      <c r="O6" s="62"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="62"/>
+      <c r="O6" s="54"/>
+      <c r="P6" s="54"/>
+      <c r="Q6" s="54"/>
       <c r="R6" s="14"/>
       <c r="S6" s="14"/>
       <c r="T6" s="14"/>
@@ -9270,30 +9315,30 @@
     </row>
     <row r="7" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14"/>
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="59"/>
-      <c r="D7" s="59"/>
-      <c r="E7" s="59"/>
-      <c r="F7" s="59" t="s">
+      <c r="C7" s="55"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55" t="s">
         <v>61</v>
       </c>
-      <c r="G7" s="59"/>
-      <c r="H7" s="59"/>
-      <c r="I7" s="59"/>
-      <c r="J7" s="59" t="s">
+      <c r="G7" s="55"/>
+      <c r="H7" s="55"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59"/>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59" t="s">
+      <c r="K7" s="55"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55" t="s">
         <v>63</v>
       </c>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="55"/>
       <c r="R7" s="14"/>
       <c r="S7" s="14"/>
       <c r="T7" s="14"/>
@@ -9353,24 +9398,24 @@
     </row>
     <row r="10" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
-      <c r="B10" s="53" t="s">
+      <c r="B10" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="52"/>
+      <c r="J10" s="52"/>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+      <c r="Q10" s="52"/>
       <c r="R10" s="14"/>
       <c r="S10" s="14"/>
       <c r="T10" s="14"/>
@@ -9380,29 +9425,29 @@
     </row>
     <row r="11" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="56" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="57"/>
-      <c r="J11" s="57"/>
-      <c r="K11" s="58">
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57">
         <f ca="1">T12</f>
-        <v>12</v>
-      </c>
-      <c r="L11" s="58"/>
-      <c r="M11" s="58"/>
-      <c r="N11" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="L11" s="57"/>
+      <c r="M11" s="57"/>
+      <c r="N11" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="O11" s="56"/>
-      <c r="P11" s="56"/>
-      <c r="Q11" s="56"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
       <c r="R11" s="14"/>
       <c r="S11" s="14"/>
       <c r="T11" s="14"/>
@@ -9412,34 +9457,34 @@
     </row>
     <row r="12" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="57"/>
-      <c r="J12" s="57"/>
-      <c r="K12" s="58">
+      <c r="C12" s="56"/>
+      <c r="D12" s="56"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="56"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57">
         <f ca="1">T13</f>
-        <v>20</v>
-      </c>
-      <c r="L12" s="58"/>
-      <c r="M12" s="58"/>
-      <c r="N12" s="56" t="s">
+        <v>10</v>
+      </c>
+      <c r="L12" s="57"/>
+      <c r="M12" s="57"/>
+      <c r="N12" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="O12" s="56"/>
-      <c r="P12" s="56"/>
-      <c r="Q12" s="56"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
       <c r="R12" s="14"/>
       <c r="S12" s="14"/>
       <c r="T12" s="17">
         <f ca="1">MIN((COUNTIFS(Log!A:A,"&gt;="&amp;TODAY()-7)/5)*30,30)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="U12" s="14"/>
       <c r="V12" s="14"/>
@@ -9447,34 +9492,34 @@
     </row>
     <row r="13" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="57"/>
-      <c r="K13" s="58">
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57">
         <f>T14</f>
         <v>4.1666666666666661</v>
       </c>
-      <c r="L13" s="58"/>
-      <c r="M13" s="58"/>
-      <c r="N13" s="56" t="s">
+      <c r="L13" s="57"/>
+      <c r="M13" s="57"/>
+      <c r="N13" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="O13" s="56"/>
-      <c r="P13" s="56"/>
-      <c r="Q13" s="56"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
       <c r="R13" s="14"/>
       <c r="S13" s="14"/>
       <c r="T13" s="17">
         <f ca="1">MAX(30-(COUNTIFS(Log!H:H,"&lt;"&amp;TODAY(),Log!G:G,"Applied")*10),0)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="U13" s="14"/>
       <c r="V13" s="14"/>
@@ -9482,29 +9527,29 @@
     </row>
     <row r="14" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="56" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="57"/>
-      <c r="H14" s="57"/>
-      <c r="I14" s="57"/>
-      <c r="J14" s="57"/>
-      <c r="K14" s="58">
+      <c r="C14" s="56"/>
+      <c r="D14" s="56"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="56"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57">
         <f>T15</f>
         <v>0</v>
       </c>
-      <c r="L14" s="58"/>
-      <c r="M14" s="58"/>
-      <c r="N14" s="56" t="s">
+      <c r="L14" s="57"/>
+      <c r="M14" s="57"/>
+      <c r="N14" s="58" t="s">
         <v>71</v>
       </c>
-      <c r="O14" s="56"/>
-      <c r="P14" s="56"/>
-      <c r="Q14" s="56"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="58"/>
+      <c r="Q14" s="58"/>
       <c r="R14" s="14"/>
       <c r="S14" s="14"/>
       <c r="T14" s="17">
@@ -9517,27 +9562,27 @@
     </row>
     <row r="15" spans="1:23" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
-      <c r="B15" s="54" t="s">
+      <c r="B15" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="54"/>
-      <c r="E15" s="54"/>
-      <c r="F15" s="54"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="54"/>
-      <c r="I15" s="54"/>
-      <c r="J15" s="54"/>
-      <c r="K15" s="55">
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="60">
         <f ca="1">T16</f>
-        <v>36.166666666666664</v>
-      </c>
-      <c r="L15" s="55"/>
-      <c r="M15" s="55"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="56"/>
-      <c r="P15" s="56"/>
-      <c r="Q15" s="56"/>
+        <v>14.166666666666666</v>
+      </c>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="58"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="58"/>
+      <c r="Q15" s="58"/>
       <c r="R15" s="14"/>
       <c r="S15" s="14"/>
       <c r="T15" s="17">
@@ -9570,7 +9615,7 @@
       <c r="S16" s="14"/>
       <c r="T16" s="17">
         <f ca="1">T12+T13+T14+T15</f>
-        <v>36.166666666666664</v>
+        <v>14.166666666666666</v>
       </c>
       <c r="U16" s="14"/>
       <c r="V16" s="14"/>
@@ -9578,24 +9623,24 @@
     </row>
     <row r="17" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="53"/>
-      <c r="F17" s="53"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="53"/>
-      <c r="J17" s="53"/>
-      <c r="K17" s="53"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="52"/>
       <c r="R17" s="14"/>
       <c r="S17" s="14"/>
       <c r="T17" s="14"/>
@@ -9902,24 +9947,24 @@
     </row>
     <row r="26" spans="1:23" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="14"/>
-      <c r="B26" s="53" t="s">
+      <c r="B26" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="53"/>
-      <c r="P26" s="53"/>
-      <c r="Q26" s="53"/>
+      <c r="C26" s="52"/>
+      <c r="D26" s="52"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="52"/>
+      <c r="G26" s="52"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="52"/>
+      <c r="J26" s="52"/>
+      <c r="K26" s="52"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="52"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="52"/>
+      <c r="P26" s="52"/>
+      <c r="Q26" s="52"/>
       <c r="R26" s="14"/>
       <c r="S26" s="14"/>
       <c r="T26" s="14"/>
@@ -9968,8 +10013,8 @@
         <v>2</v>
       </c>
       <c r="D28" s="18">
-        <f>IFERROR(C28/(COUNTA(Log!A:A)-1),0)</f>
-        <v>0.33333333333333331</v>
+        <f>IFERROR(C28/(COUNTA(Log!A:A)-2),0)</f>
+        <v>0.4</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -10001,8 +10046,8 @@
         <v>1</v>
       </c>
       <c r="D29" s="19">
-        <f>IFERROR(C29/(COUNTA(Log!A:A)-1),0)</f>
-        <v>0.16666666666666666</v>
+        <f>IFERROR(C29/(COUNTA(Log!A:A)-2),0)</f>
+        <v>0.2</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -10034,8 +10079,8 @@
         <v>1</v>
       </c>
       <c r="D30" s="18">
-        <f>IFERROR(C30/(COUNTA(Log!A:A)-1),0)</f>
-        <v>0.16666666666666666</v>
+        <f>IFERROR(C30/(COUNTA(Log!A:A)-2),0)</f>
+        <v>0.2</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
@@ -10067,7 +10112,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="19">
-        <f>IFERROR(C31/(COUNTA(Log!A:A)-1),0)</f>
+        <f>IFERROR(C31/(COUNTA(Log!A:A)-2),0)</f>
         <v>0</v>
       </c>
       <c r="E31" s="14"/>
@@ -10100,7 +10145,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="18">
-        <f>IFERROR(C32/(COUNTA(Log!A:A)-1),0)</f>
+        <f>IFERROR(C32/(COUNTA(Log!A:A)-2),0)</f>
         <v>0</v>
       </c>
       <c r="E32" s="14"/>
@@ -10133,8 +10178,8 @@
         <v>1</v>
       </c>
       <c r="D33" s="19">
-        <f>IFERROR(C33/(COUNTA(Log!A:A)-1),0)</f>
-        <v>0.16666666666666666</v>
+        <f>IFERROR(C33/(COUNTA(Log!A:A)-2),0)</f>
+        <v>0.2</v>
       </c>
       <c r="E33" s="14"/>
       <c r="F33" s="14"/>
@@ -10166,7 +10211,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="18">
-        <f>IFERROR(C34/(COUNTA(Log!A:A)-1),0)</f>
+        <f>IFERROR(C34/(COUNTA(Log!A:A)-2),0)</f>
         <v>0</v>
       </c>
       <c r="E34" s="14"/>
@@ -10195,8 +10240,8 @@
         <v>84</v>
       </c>
       <c r="C35" s="5">
-        <f>COUNTA(Log!A:A)-1</f>
-        <v>6</v>
+        <f>COUNTA(Log!A:A)-2</f>
+        <v>5</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>85</v>
@@ -10257,15 +10302,15 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
-      <c r="K37" s="53" t="s">
+      <c r="K37" s="52" t="s">
         <v>86</v>
       </c>
-      <c r="L37" s="53"/>
-      <c r="M37" s="53"/>
-      <c r="N37" s="53"/>
-      <c r="O37" s="53"/>
-      <c r="P37" s="53"/>
-      <c r="Q37" s="53"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="52"/>
+      <c r="O37" s="52"/>
+      <c r="P37" s="52"/>
+      <c r="Q37" s="52"/>
       <c r="R37" s="14"/>
       <c r="S37" s="14"/>
       <c r="T37" s="14"/>
@@ -10284,17 +10329,17 @@
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
-      <c r="K38" s="51" t="s">
+      <c r="K38" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="L38" s="51"/>
-      <c r="M38" s="51"/>
-      <c r="N38" s="51"/>
-      <c r="O38" s="52" t="s">
+      <c r="L38" s="61"/>
+      <c r="M38" s="61"/>
+      <c r="N38" s="61"/>
+      <c r="O38" s="62" t="s">
         <v>88</v>
       </c>
-      <c r="P38" s="52"/>
-      <c r="Q38" s="52"/>
+      <c r="P38" s="62"/>
+      <c r="Q38" s="62"/>
       <c r="R38" s="14"/>
       <c r="S38" s="14"/>
       <c r="T38" s="14"/>
@@ -10313,17 +10358,17 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
-      <c r="K39" s="51" t="s">
+      <c r="K39" s="61" t="s">
         <v>89</v>
       </c>
-      <c r="L39" s="51"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="51"/>
-      <c r="O39" s="52" t="s">
+      <c r="L39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="62" t="s">
         <v>90</v>
       </c>
-      <c r="P39" s="52"/>
-      <c r="Q39" s="52"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="62"/>
       <c r="R39" s="14"/>
       <c r="S39" s="14"/>
       <c r="T39" s="14"/>
@@ -10342,17 +10387,17 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
-      <c r="K40" s="51" t="s">
+      <c r="K40" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="L40" s="51"/>
-      <c r="M40" s="51"/>
-      <c r="N40" s="51"/>
-      <c r="O40" s="52" t="s">
+      <c r="L40" s="61"/>
+      <c r="M40" s="61"/>
+      <c r="N40" s="61"/>
+      <c r="O40" s="62" t="s">
         <v>92</v>
       </c>
-      <c r="P40" s="52"/>
-      <c r="Q40" s="52"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="62"/>
       <c r="R40" s="14"/>
       <c r="S40" s="14"/>
       <c r="T40" s="14"/>
@@ -11337,34 +11382,6 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="B4:Q4"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="B10:Q10"/>
-    <mergeCell ref="B11:J11"/>
-    <mergeCell ref="K11:M11"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="B12:J12"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="B13:J13"/>
-    <mergeCell ref="K13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="B14:J14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="N14:Q14"/>
-    <mergeCell ref="B15:J15"/>
-    <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N15:Q15"/>
-    <mergeCell ref="B17:Q17"/>
-    <mergeCell ref="B26:Q26"/>
     <mergeCell ref="K40:N40"/>
     <mergeCell ref="O40:Q40"/>
     <mergeCell ref="K37:Q37"/>
@@ -11372,6 +11389,34 @@
     <mergeCell ref="O38:Q38"/>
     <mergeCell ref="K39:N39"/>
     <mergeCell ref="O39:Q39"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="K15:M15"/>
+    <mergeCell ref="N15:Q15"/>
+    <mergeCell ref="B17:Q17"/>
+    <mergeCell ref="B26:Q26"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="B14:J14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="N14:Q14"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="K11:M11"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="B10:Q10"/>
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="B4:Q4"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -11386,7 +11431,9 @@
   </sheetPr>
   <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11417,14 +11464,14 @@
       <c r="F2" s="63"/>
     </row>
     <row r="4" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
     </row>
     <row r="5" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -11440,14 +11487,14 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="53"/>
-      <c r="C9" s="53"/>
-      <c r="D9" s="53"/>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
+      <c r="B9" s="52"/>
+      <c r="C9" s="52"/>
+      <c r="D9" s="52"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="52"/>
     </row>
     <row r="10" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -11521,14 +11568,14 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="A20" s="52" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-      <c r="F20" s="53"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
     </row>
     <row r="21" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
@@ -11676,14 +11723,14 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
     </row>
     <row r="31" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -11699,14 +11746,14 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="53" t="s">
+      <c r="A35" s="52" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="53"/>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53"/>
-      <c r="F35" s="53"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
     </row>
     <row r="36" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
@@ -11728,11 +11775,11 @@
     <row r="37" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="30">
         <f ca="1">TODAY()-56</f>
-        <v>46021</v>
+        <v>46026</v>
       </c>
       <c r="B37" s="30">
         <f t="shared" ref="B37:B44" ca="1" si="0">A37+6</f>
-        <v>46027</v>
+        <v>46032</v>
       </c>
       <c r="C37" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A37,Log!A:A,"&lt;="&amp;B37)</f>
@@ -11750,11 +11797,11 @@
     <row r="38" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="31">
         <f ca="1">TODAY()-49</f>
-        <v>46028</v>
+        <v>46033</v>
       </c>
       <c r="B38" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>46034</v>
+        <v>46039</v>
       </c>
       <c r="C38" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A38,Log!A:A,"&lt;="&amp;B38)</f>
@@ -11772,11 +11819,11 @@
     <row r="39" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="30">
         <f ca="1">TODAY()-42</f>
-        <v>46035</v>
+        <v>46040</v>
       </c>
       <c r="B39" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>46041</v>
+        <v>46046</v>
       </c>
       <c r="C39" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A39,Log!A:A,"&lt;="&amp;B39)</f>
@@ -11794,11 +11841,11 @@
     <row r="40" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="31">
         <f ca="1">TODAY()-35</f>
-        <v>46042</v>
+        <v>46047</v>
       </c>
       <c r="B40" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>46048</v>
+        <v>46053</v>
       </c>
       <c r="C40" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A40,Log!A:A,"&lt;="&amp;B40)</f>
@@ -11816,11 +11863,11 @@
     <row r="41" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <f ca="1">TODAY()-28</f>
-        <v>46049</v>
+        <v>46054</v>
       </c>
       <c r="B41" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>46055</v>
+        <v>46060</v>
       </c>
       <c r="C41" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A41,Log!A:A,"&lt;="&amp;B41)</f>
@@ -11838,19 +11885,19 @@
     <row r="42" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="31">
         <f ca="1">TODAY()-21</f>
-        <v>46056</v>
+        <v>46061</v>
       </c>
       <c r="B42" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>46062</v>
+        <v>46067</v>
       </c>
       <c r="C42" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A42,Log!A:A,"&lt;="&amp;B42)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D42" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A42,Log!A:A,"&lt;="&amp;B42,Log!G:G,"Interview Scheduled")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A42,Log!A:A,"&lt;="&amp;B42,Log!G:G,"Offer")</f>
@@ -11860,19 +11907,19 @@
     <row r="43" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <f ca="1">TODAY()-14</f>
-        <v>46063</v>
+        <v>46068</v>
       </c>
       <c r="B43" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>46069</v>
+        <v>46074</v>
       </c>
       <c r="C43" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A43,Log!A:A,"&lt;="&amp;B43)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D43" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A43,Log!A:A,"&lt;="&amp;B43,Log!G:G,"Interview Scheduled")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43" s="8">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A43,Log!A:A,"&lt;="&amp;B43,Log!G:G,"Offer")</f>
@@ -11882,15 +11929,15 @@
     <row r="44" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="31">
         <f ca="1">TODAY()-7</f>
-        <v>46070</v>
+        <v>46075</v>
       </c>
       <c r="B44" s="31">
         <f t="shared" ca="1" si="0"/>
-        <v>46076</v>
+        <v>46081</v>
       </c>
       <c r="C44" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A44,Log!A:A,"&lt;="&amp;B44)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" s="12">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;A44,Log!A:A,"&lt;="&amp;B44,Log!G:G,"Interview Scheduled")</f>
@@ -11924,7 +11971,9 @@
   </sheetPr>
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12311,7 +12360,9 @@
   </sheetPr>
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:K1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12343,51 +12394,51 @@
       <c r="K1" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="52" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="53"/>
-      <c r="K3" s="53"/>
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="52"/>
+      <c r="J3" s="52"/>
+      <c r="K3" s="52"/>
     </row>
     <row r="4" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="66" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="70"/>
-      <c r="C4" s="70"/>
-      <c r="D4" s="70"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="70"/>
-      <c r="G4" s="70"/>
-      <c r="H4" s="70"/>
-      <c r="I4" s="70"/>
-      <c r="J4" s="70"/>
-      <c r="K4" s="70"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
     </row>
     <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="53" t="s">
+      <c r="A6" s="52" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="53"/>
-      <c r="C6" s="53"/>
-      <c r="E6" s="53" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="E6" s="52" t="s">
         <v>119</v>
       </c>
-      <c r="F6" s="53"/>
-      <c r="H6" s="53" t="s">
+      <c r="F6" s="52"/>
+      <c r="H6" s="52" t="s">
         <v>120</v>
       </c>
-      <c r="I6" s="53"/>
-      <c r="J6" s="53"/>
-      <c r="K6" s="53"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
+      <c r="K6" s="52"/>
     </row>
     <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
@@ -12834,19 +12885,19 @@
       </c>
     </row>
     <row r="30" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="53"/>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="53"/>
+      <c r="B30" s="52"/>
+      <c r="C30" s="52"/>
+      <c r="D30" s="52"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
     </row>
     <row r="31" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
@@ -13247,13 +13298,13 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="52" t="s">
         <v>154</v>
       </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="53"/>
-      <c r="D45" s="53"/>
-      <c r="E45" s="53"/>
+      <c r="B45" s="52"/>
+      <c r="C45" s="52"/>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
     </row>
     <row r="46" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="38" t="s">
@@ -13274,25 +13325,25 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="67" t="s">
+      <c r="A48" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="B48" s="67"/>
-      <c r="C48" s="68">
+      <c r="B48" s="68"/>
+      <c r="C48" s="69">
         <f>IFERROR((TotalAchievedWeight/TotalPossibleWeight)*100,0)</f>
         <v>78.260869565217391</v>
       </c>
-      <c r="D48" s="68"/>
-      <c r="E48" s="68"/>
+      <c r="D48" s="69"/>
+      <c r="E48" s="69"/>
     </row>
     <row r="50" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="69" t="s">
+      <c r="A50" s="70" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="69"/>
-      <c r="C50" s="69"/>
-      <c r="D50" s="69"/>
-      <c r="E50" s="69"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="70"/>
+      <c r="E50" s="70"/>
     </row>
     <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="s">
@@ -13394,13 +13445,13 @@
       </c>
     </row>
     <row r="58" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="67" t="s">
         <v>160</v>
       </c>
-      <c r="B58" s="66"/>
-      <c r="C58" s="66"/>
-      <c r="D58" s="66"/>
-      <c r="E58" s="66"/>
+      <c r="B58" s="67"/>
+      <c r="C58" s="67"/>
+      <c r="D58" s="67"/>
+      <c r="E58" s="67"/>
     </row>
     <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="43" t="s">
@@ -13503,18 +13554,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A58:E58"/>
+    <mergeCell ref="A30:K30"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="A50:E50"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A58:E58"/>
-    <mergeCell ref="A30:K30"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="A50:E50"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -13536,8 +13587,8 @@
   </sheetPr>
   <dimension ref="A1:D180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81:D81"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13556,12 +13607,12 @@
       <c r="D1" s="50"/>
     </row>
     <row r="2" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
     </row>
     <row r="3" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
@@ -13596,12 +13647,12 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="53" t="s">
+      <c r="A8" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="B8" s="53"/>
-      <c r="C8" s="53"/>
-      <c r="D8" s="53"/>
+      <c r="B8" s="52"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="52"/>
     </row>
     <row r="9" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="44" t="s">
@@ -13660,12 +13711,12 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
+      <c r="A17" s="52" t="s">
         <v>182</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
     </row>
     <row r="18" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
@@ -13740,12 +13791,12 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="52" t="s">
         <v>201</v>
       </c>
-      <c r="B28" s="53"/>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
+      <c r="B28" s="52"/>
+      <c r="C28" s="52"/>
+      <c r="D28" s="52"/>
     </row>
     <row r="29" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44" t="s">
@@ -13753,7 +13804,7 @@
       </c>
       <c r="B29" s="45">
         <f ca="1">COUNTIFS(Log!A:A,"&gt;="&amp;TODAY()-7)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13762,7 +13813,7 @@
       </c>
       <c r="B30" s="45">
         <f ca="1">COUNTIFS(Log!H:H,"&lt;"&amp;TODAY(),Log!G:G,"Applied")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13784,12 +13835,12 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="53" t="s">
+      <c r="A34" s="52" t="s">
         <v>206</v>
       </c>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52"/>
+      <c r="D34" s="52"/>
     </row>
     <row r="35" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44" t="s">
@@ -13797,7 +13848,7 @@
       </c>
       <c r="B35" s="45">
         <f ca="1">MIN((COUNTIFS(Log!A:A,"&gt;="&amp;TODAY()-7)/5)*30,30)</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13806,7 +13857,7 @@
       </c>
       <c r="B36" s="45">
         <f ca="1">MAX(30-(COUNTIFS(Log!H:H,"&lt;"&amp;TODAY(),Log!G:G,"Applied")*10),0)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13833,16 +13884,16 @@
       </c>
       <c r="B39" s="45">
         <f ca="1">ScoreA+ScoreB+ScoreC+ScoreD</f>
-        <v>36.166666666666664</v>
+        <v>14.166666666666666</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="52" t="s">
         <v>212</v>
       </c>
-      <c r="B41" s="53"/>
-      <c r="C41" s="53"/>
-      <c r="D41" s="53"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
     </row>
     <row r="42" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44" t="s">
@@ -13894,12 +13945,12 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="52" t="s">
         <v>224</v>
       </c>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
+      <c r="B49" s="52"/>
+      <c r="C49" s="52"/>
+      <c r="D49" s="52"/>
     </row>
     <row r="50" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44" t="s">
@@ -13942,12 +13993,12 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="53" t="s">
+      <c r="A56" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="B56" s="53"/>
-      <c r="C56" s="53"/>
-      <c r="D56" s="53"/>
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
     </row>
     <row r="57" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="44" t="s">
@@ -13977,12 +14028,12 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="53" t="s">
+      <c r="A61" s="52" t="s">
         <v>239</v>
       </c>
-      <c r="B61" s="53"/>
-      <c r="C61" s="53"/>
-      <c r="D61" s="53"/>
+      <c r="B61" s="52"/>
+      <c r="C61" s="52"/>
+      <c r="D61" s="52"/>
     </row>
     <row r="62" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="44" t="s">
@@ -14009,12 +14060,12 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="53" t="s">
+      <c r="A66" s="52" t="s">
         <v>246</v>
       </c>
-      <c r="B66" s="53"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="53"/>
+      <c r="B66" s="52"/>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
     </row>
     <row r="67" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="44" t="s">
@@ -14073,12 +14124,12 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="53" t="s">
+      <c r="A75" s="52" t="s">
         <v>259</v>
       </c>
-      <c r="B75" s="53"/>
-      <c r="C75" s="53"/>
-      <c r="D75" s="53"/>
+      <c r="B75" s="52"/>
+      <c r="C75" s="52"/>
+      <c r="D75" s="52"/>
     </row>
     <row r="76" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
@@ -14109,12 +14160,12 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="53" t="s">
+      <c r="A80" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="B80" s="53"/>
-      <c r="C80" s="53"/>
-      <c r="D80" s="53"/>
+      <c r="B80" s="52"/>
+      <c r="C80" s="52"/>
+      <c r="D80" s="52"/>
     </row>
     <row r="81" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="71" t="s">
@@ -14910,105 +14961,6 @@
     </row>
   </sheetData>
   <mergeCells count="113">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="A56:D56"/>
-    <mergeCell ref="A61:D61"/>
-    <mergeCell ref="A66:D66"/>
-    <mergeCell ref="A75:D75"/>
-    <mergeCell ref="A80:D80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="A82:D82"/>
-    <mergeCell ref="A83:D83"/>
-    <mergeCell ref="A84:D84"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="A86:D86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="A88:D88"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A90:D90"/>
-    <mergeCell ref="A91:D91"/>
-    <mergeCell ref="A92:D92"/>
-    <mergeCell ref="A93:D93"/>
-    <mergeCell ref="A94:D94"/>
-    <mergeCell ref="A95:D95"/>
-    <mergeCell ref="A96:D96"/>
-    <mergeCell ref="A97:D97"/>
-    <mergeCell ref="A98:D98"/>
-    <mergeCell ref="A99:D99"/>
-    <mergeCell ref="A100:D100"/>
-    <mergeCell ref="A101:D101"/>
-    <mergeCell ref="A102:D102"/>
-    <mergeCell ref="A103:D103"/>
-    <mergeCell ref="A104:D104"/>
-    <mergeCell ref="A105:D105"/>
-    <mergeCell ref="A106:D106"/>
-    <mergeCell ref="A107:D107"/>
-    <mergeCell ref="A108:D108"/>
-    <mergeCell ref="A109:D109"/>
-    <mergeCell ref="A110:D110"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="A112:D112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="A114:D114"/>
-    <mergeCell ref="A115:D115"/>
-    <mergeCell ref="A116:D116"/>
-    <mergeCell ref="A117:D117"/>
-    <mergeCell ref="A118:D118"/>
-    <mergeCell ref="A119:D119"/>
-    <mergeCell ref="A120:D120"/>
-    <mergeCell ref="A121:D121"/>
-    <mergeCell ref="A122:D122"/>
-    <mergeCell ref="A123:D123"/>
-    <mergeCell ref="A124:D124"/>
-    <mergeCell ref="A125:D125"/>
-    <mergeCell ref="A126:D126"/>
-    <mergeCell ref="A127:D127"/>
-    <mergeCell ref="A128:D128"/>
-    <mergeCell ref="A129:D129"/>
-    <mergeCell ref="A130:D130"/>
-    <mergeCell ref="A131:D131"/>
-    <mergeCell ref="A132:D132"/>
-    <mergeCell ref="A133:D133"/>
-    <mergeCell ref="A134:D134"/>
-    <mergeCell ref="A135:D135"/>
-    <mergeCell ref="A136:D136"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A138:D138"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="A140:D140"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="A142:D142"/>
-    <mergeCell ref="A143:D143"/>
-    <mergeCell ref="A144:D144"/>
-    <mergeCell ref="A145:D145"/>
-    <mergeCell ref="A146:D146"/>
-    <mergeCell ref="A147:D147"/>
-    <mergeCell ref="A148:D148"/>
-    <mergeCell ref="A149:D149"/>
-    <mergeCell ref="A150:D150"/>
-    <mergeCell ref="A151:D151"/>
-    <mergeCell ref="A152:D152"/>
-    <mergeCell ref="A153:D153"/>
-    <mergeCell ref="A154:D154"/>
-    <mergeCell ref="A155:D155"/>
-    <mergeCell ref="A156:D156"/>
-    <mergeCell ref="A157:D157"/>
-    <mergeCell ref="A158:D158"/>
-    <mergeCell ref="A159:D159"/>
-    <mergeCell ref="A160:D160"/>
-    <mergeCell ref="A161:D161"/>
-    <mergeCell ref="A162:D162"/>
-    <mergeCell ref="A163:D163"/>
-    <mergeCell ref="A164:D164"/>
-    <mergeCell ref="A165:D165"/>
-    <mergeCell ref="A166:D166"/>
     <mergeCell ref="A176:D176"/>
     <mergeCell ref="A177:D177"/>
     <mergeCell ref="A178:D178"/>
@@ -15023,6 +14975,105 @@
     <mergeCell ref="A173:D173"/>
     <mergeCell ref="A174:D174"/>
     <mergeCell ref="A175:D175"/>
+    <mergeCell ref="A158:D158"/>
+    <mergeCell ref="A159:D159"/>
+    <mergeCell ref="A160:D160"/>
+    <mergeCell ref="A161:D161"/>
+    <mergeCell ref="A162:D162"/>
+    <mergeCell ref="A163:D163"/>
+    <mergeCell ref="A164:D164"/>
+    <mergeCell ref="A165:D165"/>
+    <mergeCell ref="A166:D166"/>
+    <mergeCell ref="A149:D149"/>
+    <mergeCell ref="A150:D150"/>
+    <mergeCell ref="A151:D151"/>
+    <mergeCell ref="A152:D152"/>
+    <mergeCell ref="A153:D153"/>
+    <mergeCell ref="A154:D154"/>
+    <mergeCell ref="A155:D155"/>
+    <mergeCell ref="A156:D156"/>
+    <mergeCell ref="A157:D157"/>
+    <mergeCell ref="A140:D140"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="A142:D142"/>
+    <mergeCell ref="A143:D143"/>
+    <mergeCell ref="A144:D144"/>
+    <mergeCell ref="A145:D145"/>
+    <mergeCell ref="A146:D146"/>
+    <mergeCell ref="A147:D147"/>
+    <mergeCell ref="A148:D148"/>
+    <mergeCell ref="A131:D131"/>
+    <mergeCell ref="A132:D132"/>
+    <mergeCell ref="A133:D133"/>
+    <mergeCell ref="A134:D134"/>
+    <mergeCell ref="A135:D135"/>
+    <mergeCell ref="A136:D136"/>
+    <mergeCell ref="A137:D137"/>
+    <mergeCell ref="A138:D138"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="A122:D122"/>
+    <mergeCell ref="A123:D123"/>
+    <mergeCell ref="A124:D124"/>
+    <mergeCell ref="A125:D125"/>
+    <mergeCell ref="A126:D126"/>
+    <mergeCell ref="A127:D127"/>
+    <mergeCell ref="A128:D128"/>
+    <mergeCell ref="A129:D129"/>
+    <mergeCell ref="A130:D130"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="A114:D114"/>
+    <mergeCell ref="A115:D115"/>
+    <mergeCell ref="A116:D116"/>
+    <mergeCell ref="A117:D117"/>
+    <mergeCell ref="A118:D118"/>
+    <mergeCell ref="A119:D119"/>
+    <mergeCell ref="A120:D120"/>
+    <mergeCell ref="A121:D121"/>
+    <mergeCell ref="A104:D104"/>
+    <mergeCell ref="A105:D105"/>
+    <mergeCell ref="A106:D106"/>
+    <mergeCell ref="A107:D107"/>
+    <mergeCell ref="A108:D108"/>
+    <mergeCell ref="A109:D109"/>
+    <mergeCell ref="A110:D110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="A112:D112"/>
+    <mergeCell ref="A95:D95"/>
+    <mergeCell ref="A96:D96"/>
+    <mergeCell ref="A97:D97"/>
+    <mergeCell ref="A98:D98"/>
+    <mergeCell ref="A99:D99"/>
+    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A102:D102"/>
+    <mergeCell ref="A103:D103"/>
+    <mergeCell ref="A86:D86"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="A88:D88"/>
+    <mergeCell ref="A89:D89"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A91:D91"/>
+    <mergeCell ref="A92:D92"/>
+    <mergeCell ref="A93:D93"/>
+    <mergeCell ref="A94:D94"/>
+    <mergeCell ref="A61:D61"/>
+    <mergeCell ref="A66:D66"/>
+    <mergeCell ref="A75:D75"/>
+    <mergeCell ref="A80:D80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="A82:D82"/>
+    <mergeCell ref="A83:D83"/>
+    <mergeCell ref="A84:D84"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="A56:D56"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>